<commit_message>
n gram statistics new
</commit_message>
<xml_diff>
--- a/N_GRAM/Ngram_Statistics.xlsx
+++ b/N_GRAM/Ngram_Statistics.xlsx
@@ -471,7 +471,7 @@
         <v>392179</v>
       </c>
       <c r="E2" t="n">
-        <v>387276</v>
+        <v>387275</v>
       </c>
     </row>
     <row r="3">
@@ -506,10 +506,10 @@
         <v>1.291978805042938</v>
       </c>
       <c r="D4" t="n">
-        <v>1.66835297147476</v>
+        <v>1.654744389679203</v>
       </c>
       <c r="E4" t="n">
-        <v>1.66308524153317</v>
+        <v>1.648895487702537</v>
       </c>
     </row>
     <row r="5">
@@ -544,10 +544,10 @@
         <v>1.291978805042938</v>
       </c>
       <c r="D6" t="n">
-        <v>1.66835297147476</v>
+        <v>1.654744389679203</v>
       </c>
       <c r="E6" t="n">
-        <v>1.66308524153317</v>
+        <v>1.648895487702537</v>
       </c>
     </row>
     <row r="7">
@@ -609,10 +609,10 @@
         <v>1.40171534100598</v>
       </c>
       <c r="D9" t="n">
-        <v>4.745296047483772</v>
+        <v>4.67844810573635</v>
       </c>
       <c r="E9" t="n">
-        <v>4.701583617668013</v>
+        <v>4.632017571323674</v>
       </c>
     </row>
     <row r="10">

</xml_diff>